<commit_message>
[TRY] Trying to fix the save data
</commit_message>
<xml_diff>
--- a/temp_files/difficulty.xlsx
+++ b/temp_files/difficulty.xlsx
@@ -55,10 +55,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,90 +440,90 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>level</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>conversion_num</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Aprende HTML desde CERO</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Aprende CSS desde CERO</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Medio</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Aprende Jest</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Very Hard</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>React de CERO a EXPERTO</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>hard</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Curso de JavaScript completo</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="3" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>